<commit_message>
plots for every g20 country
</commit_message>
<xml_diff>
--- a/data/summed_interventions_wide.xlsx
+++ b/data/summed_interventions_wide.xlsx
@@ -10,53 +10,6 @@
     <sheet name="Total_Interventions" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gta.evaluation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,148 +338,7 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="n">
-        <v>191</v>
-      </c>
-      <c r="C2" t="n">
-        <v>146</v>
-      </c>
-      <c r="D2" t="n">
-        <v>142</v>
-      </c>
-      <c r="E2" t="n">
-        <v>149</v>
-      </c>
-      <c r="F2" t="n">
-        <v>160</v>
-      </c>
-      <c r="G2" t="n">
-        <v>193</v>
-      </c>
-      <c r="H2" t="n">
-        <v>226</v>
-      </c>
-      <c r="I2" t="n">
-        <v>179</v>
-      </c>
-      <c r="J2" t="n">
-        <v>160</v>
-      </c>
-      <c r="K2" t="n">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="n">
-        <v>391</v>
-      </c>
-      <c r="C3" t="n">
-        <v>450</v>
-      </c>
-      <c r="D3" t="n">
-        <v>469</v>
-      </c>
-      <c r="E3" t="n">
-        <v>535</v>
-      </c>
-      <c r="F3" t="n">
-        <v>490</v>
-      </c>
-      <c r="G3" t="n">
-        <v>464</v>
-      </c>
-      <c r="H3" t="n">
-        <v>521</v>
-      </c>
-      <c r="I3" t="n">
-        <v>485</v>
-      </c>
-      <c r="J3" t="n">
-        <v>448</v>
-      </c>
-      <c r="K3" t="n">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1298</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1132</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1142</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1421</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1367</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1234</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1196</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1089</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1201</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1059</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -539,72 +351,7 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1880</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1728</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1753</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2105</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2017</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1891</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1943</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1753</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1809</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1635</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>